<commit_message>
Updated HOTCARD sheet with new entity data
</commit_message>
<xml_diff>
--- a/python/Hotcard Wave Spreadsheet.xlsx
+++ b/python/Hotcard Wave Spreadsheet.xlsx
@@ -911,14 +911,49 @@
           <t>11/26/2025</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>First National Bank</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>12345</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>FISB</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Legacy Core</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>PaymentsOne Debit</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr">
         <is>
           <t>Premium</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Dallas, TX</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>